<commit_message>
1. Sonnet 4 2. Rapise 8.5 check for OpenAi 3. OpenAi Robot startus report fixed (was false negative)
</commit_message>
<xml_diff>
--- a/FWUsefulPageObjects/TestCases/AiRobot/Robot Edits a Book/Main.rvl.xlsx
+++ b/FWUsefulPageObjects/TestCases/AiRobot/Robot Edits a Book/Main.rvl.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="330" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="331" uniqueCount="84">
   <si>
     <t>Flow</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>%WORKDIR%\Main.rvl.xlsx</t>
+  </si>
+  <si>
+    <t>Login as librarian/librarian. Press 'Login' button in the end.</t>
   </si>
 </sst>
 </file>
@@ -284,7 +287,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="644">
+  <borders count="646">
     <border>
       <left/>
       <right/>
@@ -935,11 +938,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="644">
+  <cellXfs count="646">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -1584,6 +1589,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="641" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="642" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="643" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="644" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="645" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1797,7 +1804,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection/>
@@ -1806,9 +1813,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.51171875" customWidth="true"/>
-    <col min="2" max="2" width="8.7734375" customWidth="true"/>
+    <col min="2" max="2" width="8.71875" customWidth="true"/>
     <col min="3" max="3" width="9.3359375" customWidth="true"/>
-    <col min="4" max="4" width="9.671875" customWidth="true"/>
+    <col min="4" max="4" width="9.6171875" customWidth="true"/>
     <col min="5" max="5" width="7.25390625" customWidth="true"/>
     <col min="6" max="6" width="6.6953125" customWidth="true"/>
     <col min="7" max="7" width="12.4296875" customWidth="true"/>
@@ -1863,46 +1870,52 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="370"/>
-      <c r="B3" t="s">
+      <c r="A3" s="368"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="367"/>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="369"/>
-      <c r="B4" t="s">
-        <v>23</v>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="368"/>
+      <c r="A5" s="366"/>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="367"/>
+      <c r="A6" s="373"/>
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1919,11 +1932,11 @@
         <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="366"/>
+      <c r="A7" s="372"/>
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -1940,203 +1953,161 @@
         <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="373"/>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>29</v>
-      </c>
+      <c r="A8" s="397"/>
     </row>
     <row r="9">
-      <c r="A9" s="372"/>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>30</v>
-      </c>
+      <c r="A9" s="222"/>
+      <c r="B9" s="223"/>
+      <c r="C9" s="224"/>
+      <c r="D9" s="225"/>
+      <c r="E9" s="226"/>
+      <c r="F9" s="227"/>
+      <c r="G9" s="228"/>
+      <c r="H9" s="229"/>
     </row>
     <row r="10">
-      <c r="A10" s="397"/>
+      <c r="A10" s="254"/>
+      <c r="B10" s="255"/>
+      <c r="C10" s="256"/>
+      <c r="D10" s="257"/>
+      <c r="E10" s="258"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="260"/>
+      <c r="H10" s="261"/>
     </row>
     <row r="11">
-      <c r="A11" s="222"/>
-      <c r="B11" s="223"/>
-      <c r="C11" s="224"/>
-      <c r="D11" s="225"/>
-      <c r="E11" s="226"/>
-      <c r="F11" s="227"/>
-      <c r="G11" s="228"/>
-      <c r="H11" s="229"/>
+      <c r="A11" s="262"/>
+      <c r="B11" s="263"/>
+      <c r="C11" s="264"/>
+      <c r="D11" s="265"/>
+      <c r="E11" s="266"/>
+      <c r="F11" s="267"/>
+      <c r="G11" s="268"/>
+      <c r="H11" s="269"/>
     </row>
     <row r="12">
-      <c r="A12" s="254"/>
-      <c r="B12" s="255"/>
-      <c r="C12" s="256"/>
-      <c r="D12" s="257"/>
-      <c r="E12" s="258"/>
-      <c r="F12" s="259"/>
-      <c r="G12" s="260"/>
-      <c r="H12" s="261"/>
+      <c r="A12" s="270"/>
+      <c r="B12" s="271"/>
+      <c r="C12" s="272"/>
+      <c r="D12" s="273"/>
+      <c r="E12" s="274"/>
+      <c r="F12" s="275"/>
+      <c r="G12" s="276"/>
+      <c r="H12" s="277"/>
     </row>
     <row r="13">
-      <c r="A13" s="262"/>
-      <c r="B13" s="263"/>
-      <c r="C13" s="264"/>
-      <c r="D13" s="265"/>
-      <c r="E13" s="266"/>
-      <c r="F13" s="267"/>
-      <c r="G13" s="268"/>
-      <c r="H13" s="269"/>
+      <c r="A13" s="278"/>
+      <c r="B13" s="279"/>
+      <c r="C13" s="280"/>
+      <c r="D13" s="281"/>
+      <c r="E13" s="282"/>
+      <c r="F13" s="283"/>
+      <c r="G13" s="284"/>
+      <c r="H13" s="285"/>
     </row>
     <row r="14">
-      <c r="A14" s="270"/>
-      <c r="B14" s="271"/>
-      <c r="C14" s="272"/>
-      <c r="D14" s="273"/>
-      <c r="E14" s="274"/>
-      <c r="F14" s="275"/>
-      <c r="G14" s="276"/>
-      <c r="H14" s="277"/>
+      <c r="A14" s="286"/>
+      <c r="B14" s="287"/>
+      <c r="C14" s="288"/>
+      <c r="D14" s="289"/>
+      <c r="E14" s="290"/>
+      <c r="F14" s="291"/>
+      <c r="G14" s="292"/>
+      <c r="H14" s="293"/>
     </row>
     <row r="15">
-      <c r="A15" s="278"/>
-      <c r="B15" s="279"/>
-      <c r="C15" s="280"/>
-      <c r="D15" s="281"/>
-      <c r="E15" s="282"/>
-      <c r="F15" s="283"/>
-      <c r="G15" s="284"/>
-      <c r="H15" s="285"/>
+      <c r="A15" s="294"/>
+      <c r="B15" s="295"/>
+      <c r="C15" s="296"/>
+      <c r="D15" s="297"/>
+      <c r="E15" s="298"/>
+      <c r="F15" s="299"/>
+      <c r="G15" s="300"/>
+      <c r="H15" s="301"/>
     </row>
     <row r="16">
-      <c r="A16" s="286"/>
-      <c r="B16" s="287"/>
-      <c r="C16" s="288"/>
-      <c r="D16" s="289"/>
-      <c r="E16" s="290"/>
-      <c r="F16" s="291"/>
-      <c r="G16" s="292"/>
-      <c r="H16" s="293"/>
+      <c r="A16" s="302"/>
+      <c r="B16" s="303"/>
+      <c r="C16" s="304"/>
+      <c r="D16" s="305"/>
+      <c r="E16" s="306"/>
+      <c r="F16" s="307"/>
+      <c r="G16" s="308"/>
+      <c r="H16" s="309"/>
     </row>
     <row r="17">
-      <c r="A17" s="294"/>
-      <c r="B17" s="295"/>
-      <c r="C17" s="296"/>
-      <c r="D17" s="297"/>
-      <c r="E17" s="298"/>
-      <c r="F17" s="299"/>
-      <c r="G17" s="300"/>
-      <c r="H17" s="301"/>
+      <c r="A17" s="310"/>
+      <c r="B17" s="311"/>
+      <c r="C17" s="312"/>
+      <c r="D17" s="313"/>
+      <c r="E17" s="314"/>
+      <c r="F17" s="315"/>
+      <c r="G17" s="316"/>
+      <c r="H17" s="317"/>
     </row>
     <row r="18">
-      <c r="A18" s="302"/>
-      <c r="B18" s="303"/>
-      <c r="C18" s="304"/>
-      <c r="D18" s="305"/>
-      <c r="E18" s="306"/>
-      <c r="F18" s="307"/>
-      <c r="G18" s="308"/>
-      <c r="H18" s="309"/>
+      <c r="A18" s="318"/>
+      <c r="B18" s="319"/>
+      <c r="C18" s="320"/>
+      <c r="D18" s="321"/>
+      <c r="E18" s="322"/>
+      <c r="F18" s="323"/>
+      <c r="G18" s="324"/>
+      <c r="H18" s="325"/>
     </row>
     <row r="19">
-      <c r="A19" s="310"/>
-      <c r="B19" s="311"/>
-      <c r="C19" s="312"/>
-      <c r="D19" s="313"/>
-      <c r="E19" s="314"/>
-      <c r="F19" s="315"/>
-      <c r="G19" s="316"/>
-      <c r="H19" s="317"/>
+      <c r="A19" s="326"/>
+      <c r="B19" s="327"/>
+      <c r="C19" s="328"/>
+      <c r="D19" s="329"/>
+      <c r="E19" s="330"/>
+      <c r="F19" s="331"/>
+      <c r="G19" s="332"/>
+      <c r="H19" s="333"/>
     </row>
     <row r="20">
-      <c r="A20" s="318"/>
-      <c r="B20" s="319"/>
-      <c r="C20" s="320"/>
-      <c r="D20" s="321"/>
-      <c r="E20" s="322"/>
-      <c r="F20" s="323"/>
-      <c r="G20" s="324"/>
-      <c r="H20" s="325"/>
+      <c r="A20" s="334"/>
+      <c r="B20" s="335"/>
+      <c r="C20" s="336"/>
+      <c r="D20" s="337"/>
+      <c r="E20" s="338"/>
+      <c r="F20" s="339"/>
+      <c r="G20" s="340"/>
+      <c r="H20" s="341"/>
     </row>
     <row r="21">
-      <c r="A21" s="326"/>
-      <c r="B21" s="327"/>
-      <c r="C21" s="328"/>
-      <c r="D21" s="329"/>
-      <c r="E21" s="330"/>
-      <c r="F21" s="331"/>
-      <c r="G21" s="332"/>
-      <c r="H21" s="333"/>
+      <c r="A21" s="342"/>
+      <c r="B21" s="343"/>
+      <c r="C21" s="344"/>
+      <c r="D21" s="345"/>
+      <c r="E21" s="346"/>
+      <c r="F21" s="347"/>
+      <c r="G21" s="348"/>
+      <c r="H21" s="349"/>
     </row>
     <row r="22">
-      <c r="A22" s="334"/>
-      <c r="B22" s="335"/>
-      <c r="C22" s="336"/>
-      <c r="D22" s="337"/>
-      <c r="E22" s="338"/>
-      <c r="F22" s="339"/>
-      <c r="G22" s="340"/>
-      <c r="H22" s="341"/>
+      <c r="A22" s="350"/>
+      <c r="B22" s="351"/>
+      <c r="C22" s="352"/>
+      <c r="D22" s="353"/>
+      <c r="E22" s="354"/>
+      <c r="F22" s="355"/>
+      <c r="G22" s="356"/>
+      <c r="H22" s="357"/>
     </row>
     <row r="23">
-      <c r="A23" s="342"/>
-      <c r="B23" s="343"/>
-      <c r="C23" s="344"/>
-      <c r="D23" s="345"/>
-      <c r="E23" s="346"/>
-      <c r="F23" s="347"/>
-      <c r="G23" s="348"/>
-      <c r="H23" s="349"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="350"/>
-      <c r="B24" s="351"/>
-      <c r="C24" s="352"/>
-      <c r="D24" s="353"/>
-      <c r="E24" s="354"/>
-      <c r="F24" s="355"/>
-      <c r="G24" s="356"/>
-      <c r="H24" s="357"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="358"/>
-      <c r="B25" s="359"/>
-      <c r="C25" s="360"/>
-      <c r="D25" s="361"/>
-      <c r="E25" s="362"/>
-      <c r="F25" s="363"/>
-      <c r="G25" s="364"/>
-      <c r="H25" s="365"/>
+      <c r="A23" s="358"/>
+      <c r="B23" s="359"/>
+      <c r="C23" s="360"/>
+      <c r="D23" s="361"/>
+      <c r="E23" s="362"/>
+      <c r="F23" s="363"/>
+      <c r="G23" s="364"/>
+      <c r="H23" s="365"/>
     </row>
   </sheetData>
   <tableParts/>
@@ -2145,9 +2116,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2219,355 +2192,319 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="640"/>
-      <c r="B4" t="s">
+      <c r="A4" s="638"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="637"/>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="639"/>
-      <c r="B5" t="s">
-        <v>23</v>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="638"/>
+      <c r="A6" s="636"/>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="637"/>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
+      <c r="A7" s="420"/>
+      <c r="B7" s="421"/>
+      <c r="C7" s="422"/>
+      <c r="D7" s="423"/>
+      <c r="E7" s="424"/>
+      <c r="F7" s="425"/>
+      <c r="G7" s="426"/>
+      <c r="H7" s="427"/>
     </row>
     <row r="8">
-      <c r="A8" s="636"/>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
+      <c r="A8" s="428"/>
+      <c r="B8" s="429"/>
+      <c r="C8" s="430"/>
+      <c r="D8" s="431"/>
+      <c r="E8" s="432"/>
+      <c r="F8" s="433"/>
+      <c r="G8" s="434"/>
+      <c r="H8" s="435"/>
     </row>
     <row r="9">
-      <c r="A9" s="420"/>
-      <c r="B9" s="421"/>
-      <c r="C9" s="422"/>
-      <c r="D9" s="423"/>
-      <c r="E9" s="424"/>
-      <c r="F9" s="425"/>
-      <c r="G9" s="426"/>
-      <c r="H9" s="427"/>
+      <c r="A9" s="436"/>
+      <c r="B9" s="437"/>
+      <c r="C9" s="438"/>
+      <c r="D9" s="439"/>
+      <c r="E9" s="440"/>
+      <c r="F9" s="441"/>
+      <c r="G9" s="442"/>
+      <c r="H9" s="443"/>
     </row>
     <row r="10">
-      <c r="A10" s="428"/>
-      <c r="B10" s="429"/>
-      <c r="C10" s="430"/>
-      <c r="D10" s="431"/>
-      <c r="E10" s="432"/>
-      <c r="F10" s="433"/>
-      <c r="G10" s="434"/>
-      <c r="H10" s="435"/>
+      <c r="A10" s="444"/>
+      <c r="B10" s="445"/>
+      <c r="C10" s="446"/>
+      <c r="D10" s="447"/>
+      <c r="E10" s="448"/>
+      <c r="F10" s="449"/>
+      <c r="G10" s="450"/>
+      <c r="H10" s="451"/>
     </row>
     <row r="11">
-      <c r="A11" s="436"/>
-      <c r="B11" s="437"/>
-      <c r="C11" s="438"/>
-      <c r="D11" s="439"/>
-      <c r="E11" s="440"/>
-      <c r="F11" s="441"/>
-      <c r="G11" s="442"/>
-      <c r="H11" s="443"/>
+      <c r="A11" s="452"/>
+      <c r="B11" s="453"/>
+      <c r="C11" s="454"/>
+      <c r="D11" s="455"/>
+      <c r="E11" s="456"/>
+      <c r="F11" s="457"/>
+      <c r="G11" s="458"/>
+      <c r="H11" s="459"/>
     </row>
     <row r="12">
-      <c r="A12" s="444"/>
-      <c r="B12" s="445"/>
-      <c r="C12" s="446"/>
-      <c r="D12" s="447"/>
-      <c r="E12" s="448"/>
-      <c r="F12" s="449"/>
-      <c r="G12" s="450"/>
-      <c r="H12" s="451"/>
+      <c r="A12" s="460"/>
+      <c r="B12" s="461"/>
+      <c r="C12" s="462"/>
+      <c r="D12" s="463"/>
+      <c r="E12" s="464"/>
+      <c r="F12" s="465"/>
+      <c r="G12" s="466"/>
+      <c r="H12" s="467"/>
     </row>
     <row r="13">
-      <c r="A13" s="452"/>
-      <c r="B13" s="453"/>
-      <c r="C13" s="454"/>
-      <c r="D13" s="455"/>
-      <c r="E13" s="456"/>
-      <c r="F13" s="457"/>
-      <c r="G13" s="458"/>
-      <c r="H13" s="459"/>
+      <c r="A13" s="468"/>
+      <c r="B13" s="469"/>
+      <c r="C13" s="470"/>
+      <c r="D13" s="471"/>
+      <c r="E13" s="472"/>
+      <c r="F13" s="473"/>
+      <c r="G13" s="474"/>
+      <c r="H13" s="475"/>
     </row>
     <row r="14">
-      <c r="A14" s="460"/>
-      <c r="B14" s="461"/>
-      <c r="C14" s="462"/>
-      <c r="D14" s="463"/>
-      <c r="E14" s="464"/>
-      <c r="F14" s="465"/>
-      <c r="G14" s="466"/>
-      <c r="H14" s="467"/>
+      <c r="A14" s="476"/>
+      <c r="B14" s="477"/>
+      <c r="C14" s="478"/>
+      <c r="D14" s="479"/>
+      <c r="E14" s="480"/>
+      <c r="F14" s="481"/>
+      <c r="G14" s="482"/>
+      <c r="H14" s="483"/>
     </row>
     <row r="15">
-      <c r="A15" s="468"/>
-      <c r="B15" s="469"/>
-      <c r="C15" s="470"/>
-      <c r="D15" s="471"/>
-      <c r="E15" s="472"/>
-      <c r="F15" s="473"/>
-      <c r="G15" s="474"/>
-      <c r="H15" s="475"/>
+      <c r="A15" s="484"/>
+      <c r="B15" s="485"/>
+      <c r="C15" s="486"/>
+      <c r="D15" s="487"/>
+      <c r="E15" s="488"/>
+      <c r="F15" s="489"/>
+      <c r="G15" s="490"/>
+      <c r="H15" s="491"/>
     </row>
     <row r="16">
-      <c r="A16" s="476"/>
-      <c r="B16" s="477"/>
-      <c r="C16" s="478"/>
-      <c r="D16" s="479"/>
-      <c r="E16" s="480"/>
-      <c r="F16" s="481"/>
-      <c r="G16" s="482"/>
-      <c r="H16" s="483"/>
+      <c r="A16" s="492"/>
+      <c r="B16" s="493"/>
+      <c r="C16" s="494"/>
+      <c r="D16" s="495"/>
+      <c r="E16" s="496"/>
+      <c r="F16" s="497"/>
+      <c r="G16" s="498"/>
+      <c r="H16" s="499"/>
     </row>
     <row r="17">
-      <c r="A17" s="484"/>
-      <c r="B17" s="485"/>
-      <c r="C17" s="486"/>
-      <c r="D17" s="487"/>
-      <c r="E17" s="488"/>
-      <c r="F17" s="489"/>
-      <c r="G17" s="490"/>
-      <c r="H17" s="491"/>
+      <c r="A17" s="500"/>
+      <c r="B17" s="501"/>
+      <c r="C17" s="502"/>
+      <c r="D17" s="503"/>
+      <c r="E17" s="504"/>
+      <c r="F17" s="505"/>
+      <c r="G17" s="506"/>
+      <c r="H17" s="507"/>
     </row>
     <row r="18">
-      <c r="A18" s="492"/>
-      <c r="B18" s="493"/>
-      <c r="C18" s="494"/>
-      <c r="D18" s="495"/>
-      <c r="E18" s="496"/>
-      <c r="F18" s="497"/>
-      <c r="G18" s="498"/>
-      <c r="H18" s="499"/>
+      <c r="A18" s="508"/>
+      <c r="B18" s="509"/>
+      <c r="C18" s="510"/>
+      <c r="D18" s="511"/>
+      <c r="E18" s="512"/>
+      <c r="F18" s="513"/>
+      <c r="G18" s="514"/>
+      <c r="H18" s="515"/>
     </row>
     <row r="19">
-      <c r="A19" s="500"/>
-      <c r="B19" s="501"/>
-      <c r="C19" s="502"/>
-      <c r="D19" s="503"/>
-      <c r="E19" s="504"/>
-      <c r="F19" s="505"/>
-      <c r="G19" s="506"/>
-      <c r="H19" s="507"/>
+      <c r="A19" s="516"/>
+      <c r="B19" s="517"/>
+      <c r="C19" s="518"/>
+      <c r="D19" s="519"/>
+      <c r="E19" s="520"/>
+      <c r="F19" s="521"/>
+      <c r="G19" s="522"/>
+      <c r="H19" s="523"/>
     </row>
     <row r="20">
-      <c r="A20" s="508"/>
-      <c r="B20" s="509"/>
-      <c r="C20" s="510"/>
-      <c r="D20" s="511"/>
-      <c r="E20" s="512"/>
-      <c r="F20" s="513"/>
-      <c r="G20" s="514"/>
-      <c r="H20" s="515"/>
+      <c r="A20" s="524"/>
+      <c r="B20" s="525"/>
+      <c r="C20" s="526"/>
+      <c r="D20" s="527"/>
+      <c r="E20" s="528"/>
+      <c r="F20" s="529"/>
+      <c r="G20" s="530"/>
+      <c r="H20" s="531"/>
     </row>
     <row r="21">
-      <c r="A21" s="516"/>
-      <c r="B21" s="517"/>
-      <c r="C21" s="518"/>
-      <c r="D21" s="519"/>
-      <c r="E21" s="520"/>
-      <c r="F21" s="521"/>
-      <c r="G21" s="522"/>
-      <c r="H21" s="523"/>
+      <c r="A21" s="532"/>
+      <c r="B21" s="533"/>
+      <c r="C21" s="534"/>
+      <c r="D21" s="535"/>
+      <c r="E21" s="536"/>
+      <c r="F21" s="537"/>
+      <c r="G21" s="538"/>
+      <c r="H21" s="539"/>
     </row>
     <row r="22">
-      <c r="A22" s="524"/>
-      <c r="B22" s="525"/>
-      <c r="C22" s="526"/>
-      <c r="D22" s="527"/>
-      <c r="E22" s="528"/>
-      <c r="F22" s="529"/>
-      <c r="G22" s="530"/>
-      <c r="H22" s="531"/>
+      <c r="A22" s="540"/>
+      <c r="B22" s="541"/>
+      <c r="C22" s="542"/>
+      <c r="D22" s="543"/>
+      <c r="E22" s="544"/>
+      <c r="F22" s="545"/>
+      <c r="G22" s="546"/>
+      <c r="H22" s="547"/>
     </row>
     <row r="23">
-      <c r="A23" s="532"/>
-      <c r="B23" s="533"/>
-      <c r="C23" s="534"/>
-      <c r="D23" s="535"/>
-      <c r="E23" s="536"/>
-      <c r="F23" s="537"/>
-      <c r="G23" s="538"/>
-      <c r="H23" s="539"/>
+      <c r="A23" s="548"/>
+      <c r="B23" s="549"/>
+      <c r="C23" s="550"/>
+      <c r="D23" s="551"/>
+      <c r="E23" s="552"/>
+      <c r="F23" s="553"/>
+      <c r="G23" s="554"/>
+      <c r="H23" s="555"/>
     </row>
     <row r="24">
-      <c r="A24" s="540"/>
-      <c r="B24" s="541"/>
-      <c r="C24" s="542"/>
-      <c r="D24" s="543"/>
-      <c r="E24" s="544"/>
-      <c r="F24" s="545"/>
-      <c r="G24" s="546"/>
-      <c r="H24" s="547"/>
+      <c r="A24" s="556"/>
+      <c r="B24" s="557"/>
+      <c r="C24" s="558"/>
+      <c r="D24" s="559"/>
+      <c r="E24" s="560"/>
+      <c r="F24" s="561"/>
+      <c r="G24" s="562"/>
+      <c r="H24" s="563"/>
     </row>
     <row r="25">
-      <c r="A25" s="548"/>
-      <c r="B25" s="549"/>
-      <c r="C25" s="550"/>
-      <c r="D25" s="551"/>
-      <c r="E25" s="552"/>
-      <c r="F25" s="553"/>
-      <c r="G25" s="554"/>
-      <c r="H25" s="555"/>
+      <c r="A25" s="564"/>
+      <c r="B25" s="565"/>
+      <c r="C25" s="566"/>
+      <c r="D25" s="567"/>
+      <c r="E25" s="568"/>
+      <c r="F25" s="569"/>
+      <c r="G25" s="570"/>
+      <c r="H25" s="571"/>
     </row>
     <row r="26">
-      <c r="A26" s="556"/>
-      <c r="B26" s="557"/>
-      <c r="C26" s="558"/>
-      <c r="D26" s="559"/>
-      <c r="E26" s="560"/>
-      <c r="F26" s="561"/>
-      <c r="G26" s="562"/>
-      <c r="H26" s="563"/>
+      <c r="A26" s="572"/>
+      <c r="B26" s="573"/>
+      <c r="C26" s="574"/>
+      <c r="D26" s="575"/>
+      <c r="E26" s="576"/>
+      <c r="F26" s="577"/>
+      <c r="G26" s="578"/>
+      <c r="H26" s="579"/>
     </row>
     <row r="27">
-      <c r="A27" s="564"/>
-      <c r="B27" s="565"/>
-      <c r="C27" s="566"/>
-      <c r="D27" s="567"/>
-      <c r="E27" s="568"/>
-      <c r="F27" s="569"/>
-      <c r="G27" s="570"/>
-      <c r="H27" s="571"/>
+      <c r="A27" s="580"/>
+      <c r="B27" s="581"/>
+      <c r="C27" s="582"/>
+      <c r="D27" s="583"/>
+      <c r="E27" s="584"/>
+      <c r="F27" s="585"/>
+      <c r="G27" s="586"/>
+      <c r="H27" s="587"/>
     </row>
     <row r="28">
-      <c r="A28" s="572"/>
-      <c r="B28" s="573"/>
-      <c r="C28" s="574"/>
-      <c r="D28" s="575"/>
-      <c r="E28" s="576"/>
-      <c r="F28" s="577"/>
-      <c r="G28" s="578"/>
-      <c r="H28" s="579"/>
+      <c r="A28" s="588"/>
+      <c r="B28" s="589"/>
+      <c r="C28" s="590"/>
+      <c r="D28" s="591"/>
+      <c r="E28" s="592"/>
+      <c r="F28" s="593"/>
+      <c r="G28" s="594"/>
+      <c r="H28" s="595"/>
     </row>
     <row r="29">
-      <c r="A29" s="580"/>
-      <c r="B29" s="581"/>
-      <c r="C29" s="582"/>
-      <c r="D29" s="583"/>
-      <c r="E29" s="584"/>
-      <c r="F29" s="585"/>
-      <c r="G29" s="586"/>
-      <c r="H29" s="587"/>
+      <c r="A29" s="596"/>
+      <c r="B29" s="597"/>
+      <c r="C29" s="598"/>
+      <c r="D29" s="599"/>
+      <c r="E29" s="600"/>
+      <c r="F29" s="601"/>
+      <c r="G29" s="602"/>
+      <c r="H29" s="603"/>
     </row>
     <row r="30">
-      <c r="A30" s="588"/>
-      <c r="B30" s="589"/>
-      <c r="C30" s="590"/>
-      <c r="D30" s="591"/>
-      <c r="E30" s="592"/>
-      <c r="F30" s="593"/>
-      <c r="G30" s="594"/>
-      <c r="H30" s="595"/>
+      <c r="A30" s="604"/>
+      <c r="B30" s="605"/>
+      <c r="C30" s="606"/>
+      <c r="D30" s="607"/>
+      <c r="E30" s="608"/>
+      <c r="F30" s="609"/>
+      <c r="G30" s="610"/>
+      <c r="H30" s="611"/>
     </row>
     <row r="31">
-      <c r="A31" s="596"/>
-      <c r="B31" s="597"/>
-      <c r="C31" s="598"/>
-      <c r="D31" s="599"/>
-      <c r="E31" s="600"/>
-      <c r="F31" s="601"/>
-      <c r="G31" s="602"/>
-      <c r="H31" s="603"/>
+      <c r="A31" s="612"/>
+      <c r="B31" s="613"/>
+      <c r="C31" s="614"/>
+      <c r="D31" s="615"/>
+      <c r="E31" s="616"/>
+      <c r="F31" s="617"/>
+      <c r="G31" s="618"/>
+      <c r="H31" s="619"/>
     </row>
     <row r="32">
-      <c r="A32" s="604"/>
-      <c r="B32" s="605"/>
-      <c r="C32" s="606"/>
-      <c r="D32" s="607"/>
-      <c r="E32" s="608"/>
-      <c r="F32" s="609"/>
-      <c r="G32" s="610"/>
-      <c r="H32" s="611"/>
+      <c r="A32" s="620"/>
+      <c r="B32" s="621"/>
+      <c r="C32" s="622"/>
+      <c r="D32" s="623"/>
+      <c r="E32" s="624"/>
+      <c r="F32" s="625"/>
+      <c r="G32" s="626"/>
+      <c r="H32" s="627"/>
     </row>
     <row r="33">
-      <c r="A33" s="612"/>
-      <c r="B33" s="613"/>
-      <c r="C33" s="614"/>
-      <c r="D33" s="615"/>
-      <c r="E33" s="616"/>
-      <c r="F33" s="617"/>
-      <c r="G33" s="618"/>
-      <c r="H33" s="619"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="620"/>
-      <c r="B34" s="621"/>
-      <c r="C34" s="622"/>
-      <c r="D34" s="623"/>
-      <c r="E34" s="624"/>
-      <c r="F34" s="625"/>
-      <c r="G34" s="626"/>
-      <c r="H34" s="627"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="628"/>
-      <c r="B35" s="629"/>
-      <c r="C35" s="630"/>
-      <c r="D35" s="631"/>
-      <c r="E35" s="632"/>
-      <c r="F35" s="633"/>
-      <c r="G35" s="634"/>
-      <c r="H35" s="635"/>
+      <c r="A33" s="628"/>
+      <c r="B33" s="629"/>
+      <c r="C33" s="630"/>
+      <c r="D33" s="631"/>
+      <c r="E33" s="632"/>
+      <c r="F33" s="633"/>
+      <c r="G33" s="634"/>
+      <c r="H33" s="635"/>
     </row>
   </sheetData>
   <tableParts/>

</xml_diff>